<commit_message>
added commit id to exp 1
</commit_message>
<xml_diff>
--- a/experiments/experiments_data.xlsx
+++ b/experiments/experiments_data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B2EA96-EB4E-40F8-B49A-247D3CCA974E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48938658-A9C2-4866-AD69-113ECAAAF7A0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
@@ -76,9 +76,6 @@
     <t>{'n_estimators': 500}</t>
   </si>
   <si>
-    <t>[Parallel(n_jobs=1)]: elapsed: 25.7min finished | refit on: f1_micro</t>
-  </si>
-  <si>
     <t>Tuning hyper-parameters</t>
   </si>
   <si>
@@ -95,13 +92,19 @@
   </si>
   <si>
     <t>(Sentinel full1&amp;full2, DEM, full indexes &amp; !ndbi)</t>
+  </si>
+  <si>
+    <t>https://github.com/AMNeves/AA-remotesensing-artificial-structures/commit/d0ebe71d432ffe0161586ad73b4e6104dbc6f552</t>
+  </si>
+  <si>
+    <t>[Parallel(n_jobs=1)]: elapsed: 25.7min finished | refit on: precision_weighted</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,6 +138,14 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -191,13 +202,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -217,9 +229,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Célula Ligada" xfId="2" builtinId="24"/>
+    <cellStyle name="Hiperligação" xfId="4" builtinId="8"/>
     <cellStyle name="Incorreto" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Verificar Célula" xfId="3" builtinId="23"/>
@@ -503,7 +519,7 @@
   <dimension ref="A1:R53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,7 +533,9 @@
     <col min="7" max="7" width="11.85546875" customWidth="1"/>
     <col min="8" max="8" width="12.42578125" customWidth="1"/>
     <col min="9" max="9" width="10.5703125" customWidth="1"/>
-    <col min="12" max="12" width="64.7109375" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" customWidth="1"/>
+    <col min="12" max="12" width="68.28515625" customWidth="1"/>
     <col min="13" max="13" width="45.7109375" customWidth="1"/>
     <col min="14" max="14" width="60.42578125" customWidth="1"/>
     <col min="15" max="15" width="13" customWidth="1"/>
@@ -534,7 +552,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -564,14 +582,11 @@
         <v>14</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
+        <v>20</v>
+      </c>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
@@ -585,10 +600,10 @@
         <v>10</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F2" s="3">
         <v>0.81254999999999999</v>
@@ -609,15 +624,17 @@
         <v>11</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>15</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="O2" s="3"/>
+        <v>17</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
       <c r="R2" s="3"/>
@@ -694,7 +711,7 @@
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
+      <c r="L6" s="6"/>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
@@ -1643,7 +1660,10 @@
       <c r="R53" s="3"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="O2" r:id="rId1" xr:uid="{5EB3A122-0E75-4448-B60D-35A6FD5F4B44}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
refactored training code, added kappa, conf matrix plot, and gridsearch plot
</commit_message>
<xml_diff>
--- a/experiments/experiments_data.xlsx
+++ b/experiments/experiments_data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48938658-A9C2-4866-AD69-113ECAAAF7A0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D98F1384-A6CE-419C-9BEF-42E2EADF0E40}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -91,13 +91,13 @@
     <t>Commit ID</t>
   </si>
   <si>
-    <t>(Sentinel full1&amp;full2, DEM, full indexes &amp; !ndbi)</t>
-  </si>
-  <si>
     <t>https://github.com/AMNeves/AA-remotesensing-artificial-structures/commit/d0ebe71d432ffe0161586ad73b4e6104dbc6f552</t>
   </si>
   <si>
     <t>[Parallel(n_jobs=1)]: elapsed: 25.7min finished | refit on: precision_weighted</t>
+  </si>
+  <si>
+    <t>(Sentinel full1&amp;full2, DEM, full indexes)</t>
   </si>
 </sst>
 </file>
@@ -519,7 +519,7 @@
   <dimension ref="A1:R53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,7 +603,7 @@
         <v>18</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F2" s="3">
         <v>0.81254999999999999</v>
@@ -624,7 +624,7 @@
         <v>11</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>15</v>
@@ -633,7 +633,7 @@
         <v>17</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
@@ -684,7 +684,7 @@
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="E5" s="6"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>

</xml_diff>

<commit_message>
added svm and xgboost files, adde xgboost first run scores
</commit_message>
<xml_diff>
--- a/experiments/experiments_data.xlsx
+++ b/experiments/experiments_data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D98F1384-A6CE-419C-9BEF-42E2EADF0E40}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE9C8EF-EB1C-4FD7-91A4-9A96F42FC632}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>Date</t>
   </si>
@@ -98,6 +98,15 @@
   </si>
   <si>
     <t>(Sentinel full1&amp;full2, DEM, full indexes)</t>
+  </si>
+  <si>
+    <t>GridSearchCV - XGBoost</t>
+  </si>
+  <si>
+    <t>[Parallel(n_jobs=4)]: elapsed: NaN min finished | refit on: precision_weighted</t>
+  </si>
+  <si>
+    <t>{'n_estimators': 1000}</t>
   </si>
 </sst>
 </file>
@@ -518,8 +527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,7 +544,7 @@
     <col min="9" max="9" width="10.5703125" customWidth="1"/>
     <col min="10" max="10" width="10.85546875" customWidth="1"/>
     <col min="11" max="11" width="10.140625" customWidth="1"/>
-    <col min="12" max="12" width="68.28515625" customWidth="1"/>
+    <col min="12" max="12" width="90" customWidth="1"/>
     <col min="13" max="13" width="45.7109375" customWidth="1"/>
     <col min="14" max="14" width="60.42578125" customWidth="1"/>
     <col min="15" max="15" width="13" customWidth="1"/>
@@ -620,8 +629,8 @@
       <c r="J2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="5" t="s">
-        <v>11</v>
+      <c r="K2">
+        <v>0.76380000000000003</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>22</v>
@@ -639,27 +648,58 @@
       <c r="Q2" s="3"/>
       <c r="R2" s="3"/>
     </row>
-    <row r="3" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
+    <row r="3" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <f>DATE(2019,4,27)</f>
+        <v>43582</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.73014000000000001</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0.74616000000000005</v>
+      </c>
+      <c r="H3" s="4">
+        <v>0.74616000000000005</v>
+      </c>
+      <c r="I3" s="3">
+        <v>0.73051999999999995</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3">
+        <v>0.66851000000000005</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -1662,8 +1702,9 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="O2" r:id="rId1" xr:uid="{5EB3A122-0E75-4448-B60D-35A6FD5F4B44}"/>
+    <hyperlink ref="O3" r:id="rId2" xr:uid="{E949B46C-2515-42E2-8974-FE52CCADCD72}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added fancy CV parameters to forest, made new experiments
</commit_message>
<xml_diff>
--- a/experiments/experiments_data.xlsx
+++ b/experiments/experiments_data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE9C8EF-EB1C-4FD7-91A4-9A96F42FC632}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A80B6D-1EAA-4A08-A1B8-55BFB9EFB412}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>{'n_estimators': 1000}</t>
+  </si>
+  <si>
+    <t>https://github.com/AMNeves/AA-remotesensing-artificial-structures/commit/8883a1a58c9a733c304785f08ea2c74fed38bfca</t>
   </si>
 </sst>
 </file>
@@ -528,7 +531,7 @@
   <dimension ref="A1:R53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -693,7 +696,7 @@
         <v>17</v>
       </c>
       <c r="O3" s="7" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>

</xml_diff>

<commit_message>
added boosted timseries experiment data
</commit_message>
<xml_diff>
--- a/experiments/experiments_data.xlsx
+++ b/experiments/experiments_data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F09821C2-40C8-42C6-9B7F-0533289AC57D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B322DB1-B370-4F59-BEFF-C51DC55BB170}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="99">
   <si>
     <t>Date</t>
   </si>
@@ -37,18 +37,12 @@
     <t>Features</t>
   </si>
   <si>
-    <t>ROC_AUC</t>
-  </si>
-  <si>
     <t>Algorithm</t>
   </si>
   <si>
     <t>Mapped COS full</t>
   </si>
   <si>
-    <t>NaN</t>
-  </si>
-  <si>
     <t>Kappa</t>
   </si>
   <si>
@@ -202,9 +196,6 @@
     <t>{'colsample_bytree': 0.5483193137202504, 'gamma': 0.1, 'gpu_id': 0, 'learning_rate': 0.6783980222181293, 'max_depth': 6, 'min_child_weight': 1, 'n_estimators': 1500, 'nthread': 4, 'objective': 'multi:softmax', 'predictor': 'gpu_predictor', 'tree_method': 'gpu_hist', 'verbose': 1}</t>
   </si>
   <si>
-    <t>(Sentinel full1&amp;full2, DEM, texture)</t>
-  </si>
-  <si>
     <t xml:space="preserve">           0       0.82      0.30      0.44       858</t>
   </si>
   <si>
@@ -230,13 +221,115 @@
   </si>
   <si>
     <t>Takes 2 hours to predict 18 million points</t>
+  </si>
+  <si>
+    <t>BoostedTree</t>
+  </si>
+  <si>
+    <t>20%  - unbalanced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           1       0.89      0.79      0.84     33283</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           2       0.92      0.82      0.87      2830</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           3       0.99      0.99      0.99    723933</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           4       0.98      0.96      0.97     15419</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   micro avg       0.98      0.98      0.98    775465</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   macro avg       0.94      0.89      0.92    775465</t>
+  </si>
+  <si>
+    <t>weighted avg       0.98      0.98      0.98    775465</t>
+  </si>
+  <si>
+    <t>cannot replicate full image oom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           1       0.80      0.60      0.69     33283</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           2       0.84      0.61      0.71      2830</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           3       0.98      0.99      0.99    723933</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           4       0.96      0.92      0.94     15419</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   micro avg       0.97      0.97      0.97    775465</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   macro avg       0.89      0.78      0.83    775465</t>
+  </si>
+  <si>
+    <t>weighted avg       0.97      0.97      0.97    775465</t>
+  </si>
+  <si>
+    <t>can replicate full image</t>
+  </si>
+  <si>
+    <t>(Sentinel full1&amp;full2, DEM,, full indexes, texture)</t>
+  </si>
+  <si>
+    <t>(Sentinel full1&amp;full2, full DEM, indexes, full texture)</t>
+  </si>
+  <si>
+    <t>(Sentinel full1&amp;full2, full DEM, timeseries)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           1       0.88      0.79      0.83     33283</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           2       0.91      0.82      0.86      2830</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           4       0.97      0.96      0.97     15419</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   macro avg       0.94      0.89      0.91    775465</t>
+  </si>
+  <si>
+    <t>half image mapping</t>
+  </si>
+  <si>
+    <t>SVM</t>
+  </si>
+  <si>
+    <t>100k  - unbalanced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           1       0.82      0.42      0.56       858</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           2       0.80      0.27      0.41        73</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           3       0.97      1.00      0.98     18671</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           4       0.96      0.85      0.90       398</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   macro avg       0.89      0.64      0.71     20000</t>
+  </si>
+  <si>
+    <t>slow training if huge data</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -285,6 +378,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -361,9 +462,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -377,6 +475,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="6" fillId="5" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -664,10 +765,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q62"/>
+  <dimension ref="A1:P102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="I54" sqref="I54"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H91" sqref="H91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -678,104 +779,97 @@
     <col min="4" max="4" width="26.7109375" customWidth="1"/>
     <col min="5" max="5" width="44.85546875" customWidth="1"/>
     <col min="6" max="6" width="57.28515625" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" customWidth="1"/>
-    <col min="8" max="8" width="11" customWidth="1"/>
-    <col min="9" max="9" width="107.85546875" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" customWidth="1"/>
-    <col min="12" max="12" width="113.7109375" customWidth="1"/>
-    <col min="13" max="13" width="60.42578125" customWidth="1"/>
-    <col min="14" max="14" width="13" customWidth="1"/>
+    <col min="7" max="7" width="30.7109375" customWidth="1"/>
+    <col min="8" max="8" width="248" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" customWidth="1"/>
+    <col min="11" max="11" width="113.7109375" customWidth="1"/>
+    <col min="12" max="12" width="60.42578125" customWidth="1"/>
+    <col min="13" max="13" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
         <f>DATE(2019,5,2)</f>
         <v>43587</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="E2" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2">
+        <v>10</v>
+      </c>
+      <c r="G2">
         <v>0.61850000000000005</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" s="6"/>
+      <c r="H2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="5"/>
+      <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
-      <c r="I3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="K3" s="3"/>
       <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="6"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="3"/>
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -787,16 +881,15 @@
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="5"/>
+      <c r="E5" s="4"/>
       <c r="F5" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -808,16 +901,15 @@
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
-      <c r="Q5" s="3"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -829,16 +921,15 @@
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
-      <c r="Q6" s="3"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -850,9 +941,8 @@
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -869,19 +959,18 @@
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="3"/>
-      <c r="H9" s="5"/>
+        <v>15</v>
+      </c>
+      <c r="G9" s="4"/>
+      <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
@@ -890,16 +979,15 @@
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
-      <c r="Q9" s="3"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -911,16 +999,15 @@
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -932,47 +1019,43 @@
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
         <f>DATE(2019,5,2)</f>
         <v>43587</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H12">
+        <v>10</v>
+      </c>
+      <c r="G12">
         <v>0.34860000000000002</v>
       </c>
-      <c r="I12" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="J12" s="6"/>
+      <c r="H12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I12" s="5"/>
+      <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
-      <c r="Q12" s="3"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -989,16 +1072,15 @@
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
-      <c r="Q13" s="3"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -1010,16 +1092,15 @@
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
-      <c r="Q14" s="3"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
@@ -1031,16 +1112,15 @@
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
-      <c r="Q15" s="3"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
@@ -1052,16 +1132,15 @@
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
-      <c r="Q16" s="3"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
@@ -1073,9 +1152,8 @@
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
       <c r="P17" s="3"/>
-      <c r="Q17" s="3"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -1092,16 +1170,15 @@
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
       <c r="P18" s="3"/>
-      <c r="Q18" s="3"/>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
@@ -1113,16 +1190,15 @@
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
       <c r="P19" s="3"/>
-      <c r="Q19" s="3"/>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
@@ -1134,16 +1210,15 @@
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
       <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
@@ -1155,9 +1230,8 @@
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>
       <c r="P21" s="3"/>
-      <c r="Q21" s="3"/>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1174,47 +1248,43 @@
       <c r="N22" s="3"/>
       <c r="O22" s="3"/>
       <c r="P22" s="3"/>
-      <c r="Q22" s="3"/>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" s="8">
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" s="7">
         <f>DATE(2019,5,2)</f>
         <v>43587</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H23">
+        <v>31</v>
+      </c>
+      <c r="G23">
         <v>0.38728726382437001</v>
       </c>
-      <c r="I23" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="J23" s="6"/>
+      <c r="H23" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I23" s="5"/>
+      <c r="J23" s="3"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
       <c r="P23" s="3"/>
-      <c r="Q23" s="3"/>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1231,16 +1301,15 @@
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
       <c r="P24" s="3"/>
-      <c r="Q24" s="3"/>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
@@ -1252,16 +1321,15 @@
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
       <c r="P25" s="3"/>
-      <c r="Q25" s="3"/>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
@@ -1273,16 +1341,15 @@
       <c r="N26" s="3"/>
       <c r="O26" s="3"/>
       <c r="P26" s="3"/>
-      <c r="Q26" s="3"/>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
@@ -1294,16 +1361,15 @@
       <c r="N27" s="3"/>
       <c r="O27" s="3"/>
       <c r="P27" s="3"/>
-      <c r="Q27" s="3"/>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
@@ -1315,9 +1381,8 @@
       <c r="N28" s="3"/>
       <c r="O28" s="3"/>
       <c r="P28" s="3"/>
-      <c r="Q28" s="3"/>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1334,16 +1399,15 @@
       <c r="N29" s="3"/>
       <c r="O29" s="3"/>
       <c r="P29" s="3"/>
-      <c r="Q29" s="3"/>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
@@ -1355,16 +1419,15 @@
       <c r="N30" s="3"/>
       <c r="O30" s="3"/>
       <c r="P30" s="3"/>
-      <c r="Q30" s="3"/>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
@@ -1376,16 +1439,15 @@
       <c r="N31" s="3"/>
       <c r="O31" s="3"/>
       <c r="P31" s="3"/>
-      <c r="Q31" s="3"/>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
@@ -1397,47 +1459,43 @@
       <c r="N32" s="3"/>
       <c r="O32" s="3"/>
       <c r="P32" s="3"/>
-      <c r="Q32" s="3"/>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A33" s="7">
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A33" s="8">
         <f>DATE(2019,5,2)</f>
         <v>43587</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H33">
+        <v>10</v>
+      </c>
+      <c r="G33">
         <v>0.65700000000000003</v>
       </c>
-      <c r="I33" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="J33" s="6"/>
+      <c r="H33" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I33" s="5"/>
+      <c r="J33" s="3"/>
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
       <c r="N33" s="3"/>
       <c r="O33" s="3"/>
       <c r="P33" s="3"/>
-      <c r="Q33" s="3"/>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -1454,16 +1512,15 @@
       <c r="N34" s="3"/>
       <c r="O34" s="3"/>
       <c r="P34" s="3"/>
-      <c r="Q34" s="3"/>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
       <c r="F35" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
@@ -1475,16 +1532,15 @@
       <c r="N35" s="3"/>
       <c r="O35" s="3"/>
       <c r="P35" s="3"/>
-      <c r="Q35" s="3"/>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
@@ -1496,16 +1552,15 @@
       <c r="N36" s="3"/>
       <c r="O36" s="3"/>
       <c r="P36" s="3"/>
-      <c r="Q36" s="3"/>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
@@ -1517,16 +1572,15 @@
       <c r="N37" s="3"/>
       <c r="O37" s="3"/>
       <c r="P37" s="3"/>
-      <c r="Q37" s="3"/>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
@@ -1538,9 +1592,8 @@
       <c r="N38" s="3"/>
       <c r="O38" s="3"/>
       <c r="P38" s="3"/>
-      <c r="Q38" s="3"/>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -1557,16 +1610,15 @@
       <c r="N39" s="3"/>
       <c r="O39" s="3"/>
       <c r="P39" s="3"/>
-      <c r="Q39" s="3"/>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
       <c r="F40" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
@@ -1578,16 +1630,15 @@
       <c r="N40" s="3"/>
       <c r="O40" s="3"/>
       <c r="P40" s="3"/>
-      <c r="Q40" s="3"/>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
       <c r="F41" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
@@ -1599,16 +1650,15 @@
       <c r="N41" s="3"/>
       <c r="O41" s="3"/>
       <c r="P41" s="3"/>
-      <c r="Q41" s="3"/>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
       <c r="F42" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
@@ -1620,47 +1670,43 @@
       <c r="N42" s="3"/>
       <c r="O42" s="3"/>
       <c r="P42" s="3"/>
-      <c r="Q42" s="3"/>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A43" s="7">
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A43" s="8">
         <f>DATE(2019,5,2)</f>
         <v>43587</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G43" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H43">
+        <v>10</v>
+      </c>
+      <c r="G43">
         <v>0.68879999999999997</v>
       </c>
-      <c r="I43" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="J43" s="6"/>
+      <c r="H43" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I43" s="5"/>
+      <c r="J43" s="3"/>
       <c r="K43" s="3"/>
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
       <c r="N43" s="3"/>
       <c r="O43" s="3"/>
       <c r="P43" s="3"/>
-      <c r="Q43" s="3"/>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -1677,16 +1723,15 @@
       <c r="N44" s="3"/>
       <c r="O44" s="3"/>
       <c r="P44" s="3"/>
-      <c r="Q44" s="3"/>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
       <c r="F45" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
@@ -1698,16 +1743,15 @@
       <c r="N45" s="3"/>
       <c r="O45" s="3"/>
       <c r="P45" s="3"/>
-      <c r="Q45" s="3"/>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
       <c r="F46" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
@@ -1719,16 +1763,15 @@
       <c r="N46" s="3"/>
       <c r="O46" s="3"/>
       <c r="P46" s="3"/>
-      <c r="Q46" s="3"/>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
       <c r="F47" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
@@ -1740,16 +1783,15 @@
       <c r="N47" s="3"/>
       <c r="O47" s="3"/>
       <c r="P47" s="3"/>
-      <c r="Q47" s="3"/>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
       <c r="F48" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
@@ -1761,9 +1803,8 @@
       <c r="N48" s="3"/>
       <c r="O48" s="3"/>
       <c r="P48" s="3"/>
-      <c r="Q48" s="3"/>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -1780,16 +1821,15 @@
       <c r="N49" s="3"/>
       <c r="O49" s="3"/>
       <c r="P49" s="3"/>
-      <c r="Q49" s="3"/>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
       <c r="F50" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
@@ -1801,16 +1841,15 @@
       <c r="N50" s="3"/>
       <c r="O50" s="3"/>
       <c r="P50" s="3"/>
-      <c r="Q50" s="3"/>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
       <c r="F51" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
@@ -1822,16 +1861,15 @@
       <c r="N51" s="3"/>
       <c r="O51" s="3"/>
       <c r="P51" s="3"/>
-      <c r="Q51" s="3"/>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
       <c r="F52" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
@@ -1843,81 +1881,352 @@
       <c r="N52" s="3"/>
       <c r="O52" s="3"/>
       <c r="P52" s="3"/>
-      <c r="Q52" s="3"/>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A53" s="7">
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A53" s="8">
         <f>DATE(2019,5,10)</f>
         <v>43595</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G53" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H53">
+        <v>10</v>
+      </c>
+      <c r="G53">
         <v>0.59430000000000005</v>
       </c>
+      <c r="H53" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="I53" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="J53" s="3" t="s">
-        <v>67</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="J53" s="3"/>
       <c r="K53" s="3"/>
       <c r="L53" s="3"/>
       <c r="M53" s="3"/>
       <c r="N53" s="3"/>
       <c r="O53" s="3"/>
       <c r="P53" s="3"/>
-      <c r="Q53" s="3"/>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="F55" t="s">
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F55" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F56" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F57" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F58" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="F56" t="s">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F59" s="3"/>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F60" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F61" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="F57" t="s">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F62" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="F58" t="s">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A63" s="6">
+        <f>DATE(2019,5,13)</f>
+        <v>43598</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G63">
+        <v>0.874151765582169</v>
+      </c>
+      <c r="H63" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I63" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F65" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F66" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F67" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F68" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F69" s="3"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F70" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F71" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F72" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" s="6">
+        <f>DATE(2019,5,14)</f>
+        <v>43599</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F73" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G73">
+        <v>0.76275680669844304</v>
+      </c>
+      <c r="H73" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I73" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F75" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F76" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F77" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F78" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F79" s="3"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F80" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F81" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F82" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" s="6">
+        <f>DATE(2019,5,14)</f>
+        <v>43599</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F83" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G83">
+        <v>0.87081806371922799</v>
+      </c>
+      <c r="H83" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I83" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F85" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F86" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F87" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F88" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F89" s="3"/>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F90" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F91" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F92" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A93" s="6">
+        <f>DATE(2019,5,14)</f>
+        <v>43599</v>
+      </c>
+      <c r="B93" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D93" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E93" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F93" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G93">
+        <v>0.66854971557089804</v>
+      </c>
+      <c r="H93" s="3" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="F60" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="F61" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="F62" t="s">
-        <v>64</v>
+      <c r="I93" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F95" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F96" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="97" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F97" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="98" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F98" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="99" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F99" s="3"/>
+    </row>
+    <row r="100" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F100" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="101" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F101" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="102" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F102" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed timeseries, refactored timeseries folders
</commit_message>
<xml_diff>
--- a/experiments/experiments_data.xlsx
+++ b/experiments/experiments_data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B38B7F7B-2592-454F-AA69-97C39F814865}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA69058D-B38D-4BAC-AF39-A84D10BA4AFC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="123">
   <si>
     <t>Date</t>
   </si>
@@ -383,6 +383,18 @@
   </si>
   <si>
     <t>weighted avg       0.96      0.97      0.96    775465</t>
+  </si>
+  <si>
+    <t>(timeseries Sentinel full1&amp;full2 fixed)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           1       0.77      0.70      0.73     29948</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           2       0.65      0.26      0.37     12635</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   macro avg       0.84      0.73      0.76    775465</t>
   </si>
 </sst>
 </file>
@@ -825,10 +837,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P132"/>
+  <dimension ref="A1:P142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F111" sqref="F111"/>
+    <sheetView tabSelected="1" topLeftCell="A112" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E136" sqref="E136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2481,22 +2493,90 @@
         <v>110</v>
       </c>
     </row>
-    <row r="129" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F129" s="3"/>
     </row>
-    <row r="130" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F130" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="131" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F131" s="3" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="132" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F132" s="3" t="s">
         <v>118</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A133" s="6">
+        <f>DATE(2019,5,14)</f>
+        <v>43599</v>
+      </c>
+      <c r="B133" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C133" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D133" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E133" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="F133" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G133">
+        <v>0.76100828484810101</v>
+      </c>
+      <c r="H133" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I133" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F135" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F136" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F137" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F138" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F139" s="3"/>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F140" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F141" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F142" s="3" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished aligned boosted classification
</commit_message>
<xml_diff>
--- a/experiments/experiments_data.xlsx
+++ b/experiments/experiments_data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8111220-9EF3-4E9B-8C37-BE711BE23190}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF61BE21-79EA-4D11-A1E6-494A22443AB2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="183">
   <si>
     <t>Date</t>
   </si>
@@ -539,6 +539,42 @@
   </si>
   <si>
     <t>weighted avg       0.96      0.96      0.96   4844437</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           1       0.72      0.64      0.68     28754</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           2       0.55      0.15      0.23     32557</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           3       0.95      0.99      0.97    698808</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           4       0.97      0.95      0.96     15346</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   micro avg       0.94      0.94      0.94    775465</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   macro avg       0.80      0.68      0.71    775465</t>
+  </si>
+  <si>
+    <t>weighted avg       0.93      0.94      0.93    775465</t>
+  </si>
+  <si>
+    <t>[[ 18443   1198   9091     22]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [  3444   4744  24318     51]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [  3717   2741 691992    358]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [    22     13    774  14537]]</t>
+  </si>
+  <si>
+    <t>Mapped COS full with all roads dynamic</t>
   </si>
 </sst>
 </file>
@@ -981,17 +1017,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P176"/>
+  <dimension ref="A1:P186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K175" sqref="K175"/>
+    <sheetView tabSelected="1" topLeftCell="A148" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C177" sqref="C177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.85546875" customWidth="1"/>
     <col min="2" max="2" width="35.5703125" customWidth="1"/>
-    <col min="3" max="3" width="26.5703125" customWidth="1"/>
+    <col min="3" max="3" width="38.28515625" customWidth="1"/>
     <col min="4" max="4" width="26.7109375" customWidth="1"/>
     <col min="5" max="5" width="44.85546875" customWidth="1"/>
     <col min="6" max="6" width="57.28515625" customWidth="1"/>
@@ -3011,6 +3047,82 @@
         <v>170</v>
       </c>
     </row>
+    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A177" s="6">
+        <f>DATE(2019,5,14)</f>
+        <v>43599</v>
+      </c>
+      <c r="B177" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C177" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="D177" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E177" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="F177" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G177">
+        <v>0.61704471926139004</v>
+      </c>
+      <c r="H177" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="I177" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I178" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F179" t="s">
+        <v>171</v>
+      </c>
+      <c r="I179" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F180" t="s">
+        <v>172</v>
+      </c>
+      <c r="I180" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F181" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F182" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F184" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F185" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F186" t="s">
+        <v>177</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added sentinel 2 scl results
</commit_message>
<xml_diff>
--- a/experiments/experiments_data.xlsx
+++ b/experiments/experiments_data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF61BE21-79EA-4D11-A1E6-494A22443AB2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B88DF57-F7D1-4A4F-8752-EB0C8F06BFDF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="199">
   <si>
     <t>Date</t>
   </si>
@@ -575,6 +575,54 @@
   </si>
   <si>
     <t>Mapped COS full with all roads dynamic</t>
+  </si>
+  <si>
+    <t>(timeseries Sentinel full1&amp;full2 fixed) 20x20m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           1       0.68      0.60      0.64     28761</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           2       0.51      0.14      0.22     32535</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           3       0.95      0.99      0.97    698803</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           4       0.96      0.92      0.94     15366</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   macro avg       0.78      0.66      0.69    775465</t>
+  </si>
+  <si>
+    <t>weighted avg       0.92      0.94      0.93    775465</t>
+  </si>
+  <si>
+    <t>(1210000, 133) (1210000,)</t>
+  </si>
+  <si>
+    <t>Kappa: 0.8595957654087517</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           1       0.88      0.84      0.86     64607</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           2       0.91      0.51      0.65     48215</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           3       0.97      0.99      0.98   1041100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           4       1.00      0.99      0.99     56078</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   micro avg       0.97      0.97      0.97   1210000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   macro avg       0.94      0.83      0.87   1210000</t>
+  </si>
+  <si>
+    <t>weighted avg       0.97      0.97      0.96   1210000</t>
   </si>
 </sst>
 </file>
@@ -1017,10 +1065,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P186"/>
+  <dimension ref="A1:P198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C177" sqref="C177"/>
+    <sheetView tabSelected="1" topLeftCell="I169" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K185" sqref="K185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3123,6 +3171,106 @@
         <v>177</v>
       </c>
     </row>
+    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A187" s="6">
+        <f>DATE(2019,5,14)</f>
+        <v>43599</v>
+      </c>
+      <c r="B187" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C187" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="D187" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E187" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="F187" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G187">
+        <v>0.59132469770304796</v>
+      </c>
+      <c r="H187" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="I187" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I188" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F189" t="s">
+        <v>184</v>
+      </c>
+      <c r="I189" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F190" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F191" t="s">
+        <v>186</v>
+      </c>
+      <c r="I191" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F192" t="s">
+        <v>187</v>
+      </c>
+      <c r="I192" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="193" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="I193" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="194" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F194" t="s">
+        <v>175</v>
+      </c>
+      <c r="I194" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="195" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F195" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="196" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F196" t="s">
+        <v>189</v>
+      </c>
+      <c r="I196" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="197" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="I197" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="198" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="I198" t="s">
+        <v>198</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added SGD SVM, added uncertain matrix, ran tests for SGD
</commit_message>
<xml_diff>
--- a/experiments/experiments_data.xlsx
+++ b/experiments/experiments_data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B88DF57-F7D1-4A4F-8752-EB0C8F06BFDF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2076CB0F-1465-43F6-BD9C-427F87F9C5DA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="4575" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="201">
   <si>
     <t>Date</t>
   </si>
@@ -619,10 +619,16 @@
     <t xml:space="preserve">   micro avg       0.97      0.97      0.97   1210000</t>
   </si>
   <si>
-    <t xml:space="preserve">   macro avg       0.94      0.83      0.87   1210000</t>
-  </si>
-  <si>
-    <t>weighted avg       0.97      0.97      0.96   1210000</t>
+    <t>(timeseries Sentinel full1&amp;full2 fixed) 10x10m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           1       0.70      0.63      0.66     28754</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           2       0.54      0.15      0.23     32557</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   macro avg       0.79      0.68      0.71    775465</t>
   </si>
 </sst>
 </file>
@@ -1065,10 +1071,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P198"/>
+  <dimension ref="A1:P205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I169" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K185" sqref="K185"/>
+    <sheetView tabSelected="1" topLeftCell="D187" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="G197" sqref="G197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3235,12 +3241,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="193" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I193" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="194" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F194" t="s">
         <v>175</v>
       </c>
@@ -3248,12 +3254,12 @@
         <v>195</v>
       </c>
     </row>
-    <row r="195" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F195" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="196" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F196" t="s">
         <v>189</v>
       </c>
@@ -3261,14 +3267,62 @@
         <v>196</v>
       </c>
     </row>
-    <row r="197" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="I197" t="s">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A197" s="6">
+        <f>DATE(2019,5,14)</f>
+        <v>43599</v>
+      </c>
+      <c r="B197" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C197" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="D197" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E197" s="3" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="198" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="I198" t="s">
+      <c r="F197" t="s">
+        <v>10</v>
+      </c>
+      <c r="G197">
+        <v>0.66</v>
+      </c>
+      <c r="H197" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="I197" s="3"/>
+    </row>
+    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F199" t="s">
         <v>198</v>
+      </c>
+    </row>
+    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F200" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F201" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F202" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F204" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F205" t="s">
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
optimized boosted trees, added sgd
</commit_message>
<xml_diff>
--- a/experiments/experiments_data.xlsx
+++ b/experiments/experiments_data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2076CB0F-1465-43F6-BD9C-427F87F9C5DA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F42C47-8E18-4B41-AD31-1BEF4B9CAA72}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="4575" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="220">
   <si>
     <t>Date</t>
   </si>
@@ -629,6 +629,63 @@
   </si>
   <si>
     <t xml:space="preserve">   macro avg       0.79      0.68      0.71    775465</t>
+  </si>
+  <si>
+    <t>SVM SGD</t>
+  </si>
+  <si>
+    <t>(timeseries Sentinel full2 fixed) 10x10m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           1       0.57      0.41      0.47      7188</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           2       0.19      0.25      0.21      8139</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           3       0.96      0.94      0.95    174702</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           4       0.65      0.95      0.77      3837</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   micro avg       0.89      0.89      0.89    193866</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   macro avg       0.59      0.64      0.60    193866</t>
+  </si>
+  <si>
+    <t>weighted avg       0.90      0.89      0.90    193866</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5%  - unbalanced </t>
+  </si>
+  <si>
+    <t>{'alpha': 0.2828985957487874, 'class_weight': 'balanced', 'early_stopping': True, 'l1_ratio': 0.12293886358853467, 'loss': 'perceptron', 'max_iter': 1000, 'penalty': 'l2', 'tol': 0.001}</t>
+  </si>
+  <si>
+    <t>fastest model yet 0:13:40.458629</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           1       0.42      0.69      0.52     28754</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           2       0.36      0.04      0.07     32557</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           3       0.95      0.97      0.96    698808</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           4       0.90      0.91      0.91     15346</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   micro avg       0.92      0.92      0.92    775465</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   macro avg       0.66      0.65      0.61    775465</t>
+  </si>
+  <si>
+    <t>weighted avg       0.91      0.92      0.91    775465</t>
   </si>
 </sst>
 </file>
@@ -1071,17 +1128,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P205"/>
+  <dimension ref="A1:P225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D187" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="G197" sqref="G197"/>
+    <sheetView tabSelected="1" topLeftCell="A184" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="H219" sqref="H219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.85546875" customWidth="1"/>
     <col min="2" max="2" width="35.5703125" customWidth="1"/>
-    <col min="3" max="3" width="38.28515625" customWidth="1"/>
+    <col min="3" max="3" width="41.7109375" customWidth="1"/>
     <col min="4" max="4" width="26.7109375" customWidth="1"/>
     <col min="5" max="5" width="44.85546875" customWidth="1"/>
     <col min="6" max="6" width="57.28515625" customWidth="1"/>
@@ -2225,6 +2282,9 @@
       <c r="O53" s="3"/>
       <c r="P53" s="3"/>
     </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F54" s="3"/>
+    </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F55" s="3" t="s">
         <v>56</v>
@@ -2293,6 +2353,9 @@
         <v>74</v>
       </c>
     </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F64" s="3"/>
+    </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F65" s="3" t="s">
         <v>67</v>
@@ -2361,6 +2424,9 @@
         <v>82</v>
       </c>
     </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F74" s="3"/>
+    </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F75" s="3" t="s">
         <v>75</v>
@@ -2429,6 +2495,9 @@
         <v>90</v>
       </c>
     </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F84" s="3"/>
+    </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F85" s="3" t="s">
         <v>86</v>
@@ -2497,6 +2566,9 @@
         <v>98</v>
       </c>
     </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F94" s="3"/>
+    </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F95" s="3" t="s">
         <v>93</v>
@@ -2707,6 +2779,9 @@
         <v>112</v>
       </c>
     </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F124" s="3"/>
+    </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F125" s="3" t="s">
         <v>114</v>
@@ -2775,6 +2850,9 @@
         <v>112</v>
       </c>
     </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F134" s="3"/>
+    </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F135" s="3" t="s">
         <v>120</v>
@@ -2843,6 +2921,9 @@
         <v>125</v>
       </c>
     </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F144" s="3"/>
+    </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F145" s="3" t="s">
         <v>126</v>
@@ -2862,6 +2943,9 @@
       <c r="F148" s="3" t="s">
         <v>129</v>
       </c>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F149" s="3"/>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F150" s="3" t="s">
@@ -3132,12 +3216,13 @@
       </c>
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F178" s="3"/>
       <c r="I178" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F179" t="s">
+      <c r="F179" s="3" t="s">
         <v>171</v>
       </c>
       <c r="I179" t="s">
@@ -3145,7 +3230,7 @@
       </c>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F180" t="s">
+      <c r="F180" s="3" t="s">
         <v>172</v>
       </c>
       <c r="I180" t="s">
@@ -3153,27 +3238,30 @@
       </c>
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F181" t="s">
+      <c r="F181" s="3" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F182" t="s">
+      <c r="F182" s="3" t="s">
         <v>174</v>
       </c>
     </row>
+    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F183" s="3"/>
+    </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F184" t="s">
+      <c r="F184" s="3" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F185" t="s">
+      <c r="F185" s="3" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F186" t="s">
+      <c r="F186" s="3" t="s">
         <v>177</v>
       </c>
     </row>
@@ -3208,12 +3296,13 @@
       </c>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F188" s="3"/>
       <c r="I188" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F189" t="s">
+      <c r="F189" s="3" t="s">
         <v>184</v>
       </c>
       <c r="I189" t="s">
@@ -3221,12 +3310,12 @@
       </c>
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F190" t="s">
+      <c r="F190" s="3" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F191" t="s">
+      <c r="F191" s="3" t="s">
         <v>186</v>
       </c>
       <c r="I191" t="s">
@@ -3234,7 +3323,7 @@
       </c>
     </row>
     <row r="192" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F192" t="s">
+      <c r="F192" s="3" t="s">
         <v>187</v>
       </c>
       <c r="I192" t="s">
@@ -3242,12 +3331,13 @@
       </c>
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F193" s="3"/>
       <c r="I193" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="194" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F194" t="s">
+      <c r="F194" s="3" t="s">
         <v>175</v>
       </c>
       <c r="I194" t="s">
@@ -3255,12 +3345,12 @@
       </c>
     </row>
     <row r="195" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F195" t="s">
+      <c r="F195" s="3" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="196" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F196" t="s">
+      <c r="F196" s="3" t="s">
         <v>189</v>
       </c>
       <c r="I196" t="s">
@@ -3284,7 +3374,7 @@
       <c r="E197" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="F197" t="s">
+      <c r="F197" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G197">
@@ -3295,34 +3385,182 @@
       </c>
       <c r="I197" s="3"/>
     </row>
+    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F198" s="3"/>
+    </row>
     <row r="199" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F199" t="s">
+      <c r="F199" s="3" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="200" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F200" t="s">
+      <c r="F200" s="3" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="201" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F201" t="s">
+      <c r="F201" s="3" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="202" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F202" t="s">
+      <c r="F202" s="3" t="s">
         <v>174</v>
       </c>
     </row>
+    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F203" s="3"/>
+    </row>
     <row r="204" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F204" t="s">
+      <c r="F204" s="3" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="205" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F205" t="s">
+      <c r="F205" s="3" t="s">
         <v>200</v>
+      </c>
+    </row>
+    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A206" s="6">
+        <f>DATE(2019,5,24)</f>
+        <v>43609</v>
+      </c>
+      <c r="B206" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="C206" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="D206" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="E206" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="F206" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G206">
+        <v>0.46</v>
+      </c>
+      <c r="H206" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="I206" s="3" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F207" s="3"/>
+    </row>
+    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F208" s="3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F209" s="3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F210" s="3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F211" s="3" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F212" s="3"/>
+    </row>
+    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F213" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F214" s="3" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F215" s="3" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A216" s="6">
+        <f>DATE(2019,5,24)</f>
+        <v>43609</v>
+      </c>
+      <c r="B216" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="C216" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="D216" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="E216" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="F216" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G216">
+        <v>0.51</v>
+      </c>
+      <c r="H216" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="I216" s="3" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F217" s="3"/>
+    </row>
+    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F218" s="3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F219" s="3" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F220" s="3" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F221" s="3" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F222" s="3"/>
+    </row>
+    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F223" s="3" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F224" s="3" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="225" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F225" s="3" t="s">
+        <v>219</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added run final test file
</commit_message>
<xml_diff>
--- a/experiments/experiments_data.xlsx
+++ b/experiments/experiments_data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE0D5F94-1F40-4D8B-8078-268BBCFBFC45}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6886F7-6715-43A4-9A35-51C96681A16D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -890,12 +890,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Correto" xfId="4" builtinId="26"/>
-    <cellStyle name="Hiperligação" xfId="3" builtinId="8"/>
-    <cellStyle name="Incorreto" xfId="1" builtinId="27"/>
-    <cellStyle name="Neutro" xfId="5" builtinId="28"/>
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Check Cell" xfId="2" builtinId="23"/>
+    <cellStyle name="Good" xfId="4" builtinId="26"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
+    <cellStyle name="Neutral" xfId="5" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Verificar Célula" xfId="2" builtinId="23"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1175,28 +1175,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P252"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A217" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="H250" sqref="H250"/>
+    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="28.85546875" customWidth="1"/>
-    <col min="2" max="2" width="35.5703125" customWidth="1"/>
-    <col min="3" max="3" width="41.7109375" customWidth="1"/>
-    <col min="4" max="4" width="26.7109375" customWidth="1"/>
-    <col min="5" max="5" width="44.85546875" customWidth="1"/>
-    <col min="6" max="6" width="57.28515625" customWidth="1"/>
-    <col min="7" max="7" width="30.7109375" customWidth="1"/>
+    <col min="1" max="1" width="28.86328125" customWidth="1"/>
+    <col min="2" max="2" width="35.59765625" customWidth="1"/>
+    <col min="3" max="3" width="41.73046875" customWidth="1"/>
+    <col min="4" max="4" width="26.73046875" customWidth="1"/>
+    <col min="5" max="5" width="44.86328125" customWidth="1"/>
+    <col min="6" max="6" width="57.265625" customWidth="1"/>
+    <col min="7" max="7" width="30.73046875" customWidth="1"/>
     <col min="8" max="8" width="248" customWidth="1"/>
-    <col min="9" max="9" width="19.42578125" customWidth="1"/>
-    <col min="10" max="10" width="10.140625" customWidth="1"/>
-    <col min="11" max="11" width="113.7109375" customWidth="1"/>
-    <col min="12" max="12" width="60.42578125" customWidth="1"/>
+    <col min="9" max="9" width="19.3984375" customWidth="1"/>
+    <col min="10" max="10" width="10.1328125" customWidth="1"/>
+    <col min="11" max="11" width="113.73046875" customWidth="1"/>
+    <col min="12" max="12" width="60.3984375" customWidth="1"/>
     <col min="13" max="13" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1225,7 +1225,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A2" s="8">
         <f>DATE(2019,5,2)</f>
         <v>43587</v>
@@ -1256,7 +1256,7 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -1270,7 +1270,7 @@
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A4" s="2"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -1290,7 +1290,7 @@
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -1310,7 +1310,7 @@
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -1330,7 +1330,7 @@
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -1350,7 +1350,7 @@
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -1368,7 +1368,7 @@
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -1388,7 +1388,7 @@
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -1408,7 +1408,7 @@
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -1428,7 +1428,7 @@
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A12" s="8">
         <f>DATE(2019,5,2)</f>
         <v>43587</v>
@@ -1463,7 +1463,7 @@
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -1481,7 +1481,7 @@
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -1501,7 +1501,7 @@
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -1521,7 +1521,7 @@
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -1541,7 +1541,7 @@
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -1561,7 +1561,7 @@
       <c r="O17" s="3"/>
       <c r="P17" s="3"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -1579,7 +1579,7 @@
       <c r="O18" s="3"/>
       <c r="P18" s="3"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -1599,7 +1599,7 @@
       <c r="O19" s="3"/>
       <c r="P19" s="3"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1619,7 +1619,7 @@
       <c r="O20" s="3"/>
       <c r="P20" s="3"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1639,7 +1639,7 @@
       <c r="O21" s="3"/>
       <c r="P21" s="3"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1657,7 +1657,7 @@
       <c r="O22" s="3"/>
       <c r="P22" s="3"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A23" s="7">
         <f>DATE(2019,5,2)</f>
         <v>43587</v>
@@ -1692,7 +1692,7 @@
       <c r="O23" s="3"/>
       <c r="P23" s="3"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1710,7 +1710,7 @@
       <c r="O24" s="3"/>
       <c r="P24" s="3"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1730,7 +1730,7 @@
       <c r="O25" s="3"/>
       <c r="P25" s="3"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1750,7 +1750,7 @@
       <c r="O26" s="3"/>
       <c r="P26" s="3"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1770,7 +1770,7 @@
       <c r="O27" s="3"/>
       <c r="P27" s="3"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1790,7 +1790,7 @@
       <c r="O28" s="3"/>
       <c r="P28" s="3"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1808,7 +1808,7 @@
       <c r="O29" s="3"/>
       <c r="P29" s="3"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1828,7 +1828,7 @@
       <c r="O30" s="3"/>
       <c r="P30" s="3"/>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1848,7 +1848,7 @@
       <c r="O31" s="3"/>
       <c r="P31" s="3"/>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1868,7 +1868,7 @@
       <c r="O32" s="3"/>
       <c r="P32" s="3"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A33" s="8">
         <f>DATE(2019,5,2)</f>
         <v>43587</v>
@@ -1903,7 +1903,7 @@
       <c r="O33" s="3"/>
       <c r="P33" s="3"/>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -1921,7 +1921,7 @@
       <c r="O34" s="3"/>
       <c r="P34" s="3"/>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -1941,7 +1941,7 @@
       <c r="O35" s="3"/>
       <c r="P35" s="3"/>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -1961,7 +1961,7 @@
       <c r="O36" s="3"/>
       <c r="P36" s="3"/>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -1981,7 +1981,7 @@
       <c r="O37" s="3"/>
       <c r="P37" s="3"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -2001,7 +2001,7 @@
       <c r="O38" s="3"/>
       <c r="P38" s="3"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -2019,7 +2019,7 @@
       <c r="O39" s="3"/>
       <c r="P39" s="3"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -2039,7 +2039,7 @@
       <c r="O40" s="3"/>
       <c r="P40" s="3"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -2059,7 +2059,7 @@
       <c r="O41" s="3"/>
       <c r="P41" s="3"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -2079,7 +2079,7 @@
       <c r="O42" s="3"/>
       <c r="P42" s="3"/>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A43" s="8">
         <f>DATE(2019,5,2)</f>
         <v>43587</v>
@@ -2114,7 +2114,7 @@
       <c r="O43" s="3"/>
       <c r="P43" s="3"/>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -2132,7 +2132,7 @@
       <c r="O44" s="3"/>
       <c r="P44" s="3"/>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -2152,7 +2152,7 @@
       <c r="O45" s="3"/>
       <c r="P45" s="3"/>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -2172,7 +2172,7 @@
       <c r="O46" s="3"/>
       <c r="P46" s="3"/>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -2192,7 +2192,7 @@
       <c r="O47" s="3"/>
       <c r="P47" s="3"/>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -2212,7 +2212,7 @@
       <c r="O48" s="3"/>
       <c r="P48" s="3"/>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -2230,7 +2230,7 @@
       <c r="O49" s="3"/>
       <c r="P49" s="3"/>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
@@ -2250,7 +2250,7 @@
       <c r="O50" s="3"/>
       <c r="P50" s="3"/>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -2270,7 +2270,7 @@
       <c r="O51" s="3"/>
       <c r="P51" s="3"/>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -2290,7 +2290,7 @@
       <c r="O52" s="3"/>
       <c r="P52" s="3"/>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A53" s="8">
         <f>DATE(2019,5,10)</f>
         <v>43595</v>
@@ -2327,48 +2327,48 @@
       <c r="O53" s="3"/>
       <c r="P53" s="3"/>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.45">
       <c r="F54" s="3"/>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.45">
       <c r="F55" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.45">
       <c r="F56" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.45">
       <c r="F57" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.45">
       <c r="F58" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.45">
       <c r="F59" s="3"/>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.45">
       <c r="F60" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.45">
       <c r="F61" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.45">
       <c r="F62" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A63" s="6">
         <f>DATE(2019,5,13)</f>
         <v>43598</v>
@@ -2398,48 +2398,48 @@
         <v>74</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.45">
       <c r="F64" s="3"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F65" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F66" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F67" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F68" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F69" s="3"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F70" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F71" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F72" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A73" s="6">
         <f>DATE(2019,5,14)</f>
         <v>43599</v>
@@ -2469,48 +2469,48 @@
         <v>82</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F74" s="3"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F75" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F76" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F77" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F78" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F79" s="3"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F80" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F81" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F82" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A83" s="6">
         <f>DATE(2019,5,14)</f>
         <v>43599</v>
@@ -2540,48 +2540,48 @@
         <v>90</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F84" s="3"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F85" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F86" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F87" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F88" s="3" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F89" s="3"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F90" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F91" s="3" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F92" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A93" s="6">
         <f>DATE(2019,5,14)</f>
         <v>43599</v>
@@ -2611,48 +2611,48 @@
         <v>98</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F94" s="3"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F95" s="3" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F96" s="3" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F97" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F98" s="3" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F99" s="3"/>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F100" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F101" s="3" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F102" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A103" s="6">
         <f>DATE(2019,5,14)</f>
         <v>43599</v>
@@ -2682,48 +2682,48 @@
         <v>105</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F104" s="3"/>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F105" s="3" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F106" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F107" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F108" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F109" s="3"/>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F110" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F111" s="3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F112" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A113" s="6">
         <f>DATE(2019,5,14)</f>
         <v>43599</v>
@@ -2753,48 +2753,48 @@
         <v>112</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F114" s="3"/>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F115" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F116" s="3" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F117" s="3" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F118" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F119" s="3"/>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F120" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F121" s="3" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F122" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A123" s="6">
         <f>DATE(2019,5,14)</f>
         <v>43599</v>
@@ -2824,48 +2824,48 @@
         <v>112</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F124" s="3"/>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F125" s="3" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F126" s="3" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F127" s="3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F128" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F129" s="3"/>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F130" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F131" s="3" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F132" s="3" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A133" s="6">
         <f>DATE(2019,5,14)</f>
         <v>43599</v>
@@ -2895,48 +2895,48 @@
         <v>112</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F134" s="3"/>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F135" s="3" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F136" s="3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F137" s="3" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F138" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F139" s="3"/>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F140" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F141" s="3" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F142" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A143" s="6">
         <f>DATE(2019,5,14)</f>
         <v>43599</v>
@@ -2966,48 +2966,48 @@
         <v>125</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F144" s="3"/>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F145" s="3" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F146" s="3" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F147" s="3" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F148" s="3" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F149" s="3"/>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F150" s="3" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F151" s="3" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F152" s="3" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A153" s="6">
         <f>DATE(2019,5,14)</f>
         <v>43599</v>
@@ -3037,48 +3037,48 @@
         <v>141</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F154" s="3"/>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F155" s="3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F156" s="3" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F157" s="3" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F158" s="3" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F159" s="3"/>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F160" s="3" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.45">
       <c r="F161" s="3" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.45">
       <c r="F162" s="3" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A163" s="6">
         <f>DATE(2019,5,14)</f>
         <v>43599</v>
@@ -3111,7 +3111,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.45">
       <c r="F164" s="3" t="s">
         <v>10</v>
       </c>
@@ -3120,7 +3120,7 @@
       </c>
       <c r="K164" s="3"/>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.45">
       <c r="F165" s="3" t="s">
         <v>143</v>
       </c>
@@ -3131,7 +3131,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.45">
       <c r="F166" s="3" t="s">
         <v>144</v>
       </c>
@@ -3142,7 +3142,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.45">
       <c r="F167" s="3" t="s">
         <v>145</v>
       </c>
@@ -3153,7 +3153,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.45">
       <c r="F168" s="3" t="s">
         <v>146</v>
       </c>
@@ -3164,7 +3164,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.45">
       <c r="F169" s="3" t="s">
         <v>147</v>
       </c>
@@ -3175,7 +3175,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.45">
       <c r="F170" s="3" t="s">
         <v>148</v>
       </c>
@@ -3186,7 +3186,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.45">
       <c r="F171" s="3" t="s">
         <v>149</v>
       </c>
@@ -3194,7 +3194,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.45">
       <c r="F172" s="3" t="s">
         <v>150</v>
       </c>
@@ -3202,11 +3202,11 @@
         <v>167</v>
       </c>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.45">
       <c r="F173" s="3"/>
       <c r="K173" s="3"/>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.45">
       <c r="F174" s="3" t="s">
         <v>79</v>
       </c>
@@ -3214,7 +3214,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.45">
       <c r="F175" s="3" t="s">
         <v>151</v>
       </c>
@@ -3222,7 +3222,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.45">
       <c r="F176" s="3" t="s">
         <v>118</v>
       </c>
@@ -3230,7 +3230,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A177" s="6">
         <f>DATE(2019,5,14)</f>
         <v>43599</v>
@@ -3260,13 +3260,13 @@
         <v>178</v>
       </c>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F178" s="3"/>
       <c r="I178" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F179" s="3" t="s">
         <v>171</v>
       </c>
@@ -3274,7 +3274,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F180" s="3" t="s">
         <v>172</v>
       </c>
@@ -3282,35 +3282,35 @@
         <v>181</v>
       </c>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F181" s="3" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F182" s="3" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F183" s="3"/>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F184" s="3" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F185" s="3" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F186" s="3" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A187" s="6">
         <f>DATE(2019,5,14)</f>
         <v>43599</v>
@@ -3340,13 +3340,13 @@
         <v>190</v>
       </c>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F188" s="3"/>
       <c r="I188" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F189" s="3" t="s">
         <v>184</v>
       </c>
@@ -3354,12 +3354,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F190" s="3" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F191" s="3" t="s">
         <v>186</v>
       </c>
@@ -3367,7 +3367,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F192" s="3" t="s">
         <v>187</v>
       </c>
@@ -3375,13 +3375,13 @@
         <v>193</v>
       </c>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F193" s="3"/>
       <c r="I193" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F194" s="3" t="s">
         <v>175</v>
       </c>
@@ -3389,12 +3389,12 @@
         <v>195</v>
       </c>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F195" s="3" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F196" s="3" t="s">
         <v>189</v>
       </c>
@@ -3402,7 +3402,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A197" s="6">
         <f>DATE(2019,5,14)</f>
         <v>43599</v>
@@ -3430,43 +3430,43 @@
       </c>
       <c r="I197" s="3"/>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F198" s="3"/>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F199" s="3" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F200" s="3" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F201" s="3" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F202" s="3" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F203" s="3"/>
     </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F204" s="3" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F205" s="3" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A206" s="6">
         <f>DATE(2019,5,24)</f>
         <v>43609</v>
@@ -3496,48 +3496,48 @@
         <v>212</v>
       </c>
     </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F207" s="3"/>
     </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F208" s="3" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F209" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F210" s="3" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F211" s="3" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F212" s="3"/>
     </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F213" s="3" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F214" s="3" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F215" s="3" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A216" s="6">
         <f>DATE(2019,5,24)</f>
         <v>43609</v>
@@ -3567,48 +3567,48 @@
         <v>212</v>
       </c>
     </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F217" s="3"/>
     </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F218" s="3" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F219" s="3" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F220" s="3" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F221" s="3" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F222" s="3"/>
     </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F223" s="3" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F224" s="3" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.45">
       <c r="F225" s="3" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A226" s="6">
         <f>DATE(2019,7,6)</f>
         <v>43652</v>
@@ -3638,43 +3638,43 @@
         <v>224</v>
       </c>
     </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:10" x14ac:dyDescent="0.45">
       <c r="F227" s="3"/>
     </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:10" x14ac:dyDescent="0.45">
       <c r="F228" s="3" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:10" x14ac:dyDescent="0.45">
       <c r="F229" s="3" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:10" x14ac:dyDescent="0.45">
       <c r="F230" s="3" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:10" x14ac:dyDescent="0.45">
       <c r="F231" s="3"/>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.45">
       <c r="F232" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:10" x14ac:dyDescent="0.45">
       <c r="F233" s="3" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:10" x14ac:dyDescent="0.45">
       <c r="F234" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A235" s="6">
         <f>DATE(2019,7,8)</f>
         <v>43654</v>
@@ -3701,43 +3701,43 @@
         <v>230</v>
       </c>
     </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:10" x14ac:dyDescent="0.45">
       <c r="F236" s="3"/>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:10" x14ac:dyDescent="0.45">
       <c r="F237" s="3" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:10" x14ac:dyDescent="0.45">
       <c r="F238" s="3" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:10" x14ac:dyDescent="0.45">
       <c r="F239" s="3" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:10" x14ac:dyDescent="0.45">
       <c r="F240" s="3"/>
     </row>
-    <row r="241" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:8" x14ac:dyDescent="0.45">
       <c r="F241" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="242" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:8" x14ac:dyDescent="0.45">
       <c r="F242" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="243" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:8" x14ac:dyDescent="0.45">
       <c r="F243" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="244" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A244" s="6">
         <f>DATE(2019,7,8)</f>
         <v>43654</v>
@@ -3764,38 +3764,38 @@
         <v>48</v>
       </c>
     </row>
-    <row r="245" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:8" x14ac:dyDescent="0.45">
       <c r="F245" s="3"/>
     </row>
-    <row r="246" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:8" x14ac:dyDescent="0.45">
       <c r="F246" s="3" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="247" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:8" x14ac:dyDescent="0.45">
       <c r="F247" s="3" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="248" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:8" x14ac:dyDescent="0.45">
       <c r="F248" s="3" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="249" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:8" x14ac:dyDescent="0.45">
       <c r="F249" s="3"/>
     </row>
-    <row r="250" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:8" x14ac:dyDescent="0.45">
       <c r="F250" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="251" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:8" x14ac:dyDescent="0.45">
       <c r="F251" s="3" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="252" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:8" x14ac:dyDescent="0.45">
       <c r="F252" s="3" t="s">
         <v>81</v>
       </c>

</xml_diff>